<commit_message>
Class Diagram update and postman collections
</commit_message>
<xml_diff>
--- a/documentation/check-list.xlsx
+++ b/documentation/check-list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\m_pro\JAVA\rebate-service\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48A5A050-9EA0-495D-81BC-5228C6D00F48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5FB1D0B-B2A1-4751-B590-995048883070}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{74E44C4B-463E-4910-A3BC-B2F9A687D0EA}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
   <si>
     <t>Feature Name</t>
   </si>
@@ -120,6 +120,9 @@
   </si>
   <si>
     <t>Logging</t>
+  </si>
+  <si>
+    <t>Partial</t>
   </si>
 </sst>
 </file>
@@ -539,10 +542,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7BFA97E-B006-4F67-80DF-04E7C981D671}">
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -551,7 +554,7 @@
     <col min="5" max="5" width="34" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -565,7 +568,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -579,7 +582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -593,7 +596,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -606,8 +609,11 @@
       <c r="F4" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -621,7 +627,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -635,7 +641,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -646,7 +652,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -657,7 +663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -668,7 +674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -679,44 +685,44 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
       <c r="B11" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>27</v>
       </c>
       <c r="B12" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>24</v>
       </c>
       <c r="B13" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>25</v>
       </c>
       <c r="B14" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -727,7 +733,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -735,7 +741,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -743,7 +749,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -751,7 +757,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -759,7 +765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -767,40 +773,43 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>22</v>
       </c>
       <c r="B22" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B25" s="2" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B27" s="2" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B28" s="2" t="b">
         <v>0</v>
       </c>

</xml_diff>